<commit_message>
fix slope math error
error is t_m math fixed
</commit_message>
<xml_diff>
--- a/Worksheets/Motor Plots.xlsx
+++ b/Worksheets/Motor Plots.xlsx
@@ -833,8 +833,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="72832512"/>
-        <c:axId val="72834048"/>
+        <c:axId val="73457664"/>
+        <c:axId val="73459968"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -1490,11 +1490,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="207210752"/>
-        <c:axId val="173300736"/>
+        <c:axId val="73595136"/>
+        <c:axId val="73593600"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="72832512"/>
+        <c:axId val="73457664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1508,12 +1508,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72834048"/>
+        <c:crossAx val="73459968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72834048"/>
+        <c:axId val="73459968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1528,12 +1528,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="72832512"/>
+        <c:crossAx val="73457664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="173300736"/>
+        <c:axId val="73593600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1543,12 +1543,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="207210752"/>
+        <c:crossAx val="73595136"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="207210752"/>
+        <c:axId val="73595136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,7 +1558,8 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="173300736"/>
+        <c:crossAx val="73593600"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
@@ -2917,11 +2918,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="74616192"/>
-        <c:axId val="74614656"/>
+        <c:axId val="74434432"/>
+        <c:axId val="74601984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74616192"/>
+        <c:axId val="74434432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2935,12 +2936,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74614656"/>
+        <c:crossAx val="74601984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74614656"/>
+        <c:axId val="74601984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2961,7 +2962,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74616192"/>
+        <c:crossAx val="74434432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4964,8 +4965,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="74703232"/>
-        <c:axId val="74705152"/>
+        <c:axId val="77266304"/>
+        <c:axId val="131992960"/>
       </c:scatterChart>
       <c:scatterChart>
         <c:scatterStyle val="smoothMarker"/>
@@ -5621,11 +5622,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="75143040"/>
-        <c:axId val="75141504"/>
+        <c:axId val="163669888"/>
+        <c:axId val="163668352"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="74703232"/>
+        <c:axId val="77266304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5640,12 +5641,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74705152"/>
+        <c:crossAx val="131992960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="74705152"/>
+        <c:axId val="131992960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5660,12 +5661,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74703232"/>
+        <c:crossAx val="77266304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75141504"/>
+        <c:axId val="163668352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5675,12 +5676,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75143040"/>
+        <c:crossAx val="163669888"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="75143040"/>
+        <c:axId val="163669888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5690,7 +5691,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75141504"/>
+        <c:crossAx val="163668352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6099,7 +6100,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6157,7 +6158,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <f>(points-Stall_Torque)/(points-0)</f>
+        <f>(Stall_Torque-0)/(points-0)</f>
         <v>0.5</v>
       </c>
     </row>
@@ -6277,11 +6278,11 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <f>E2/Scale_plot</f>
+        <f t="shared" ref="G2:G33" si="0">E2/Scale_plot</f>
         <v>0</v>
       </c>
       <c r="H2">
-        <f>F2/Scale_plot</f>
+        <f t="shared" ref="H2:H33" si="1">F2/Scale_plot</f>
         <v>0</v>
       </c>
     </row>
@@ -6302,19 +6303,19 @@
         <v>128.69999999999999</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E66" si="0">B3*D3</f>
+        <f t="shared" ref="E3:E66" si="2">B3*D3</f>
         <v>64.349999999999994</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F66" si="1">E3/C3</f>
+        <f t="shared" ref="F3:F66" si="3">E3/C3</f>
         <v>370.89337175792508</v>
       </c>
       <c r="G3">
-        <f>E3/Scale_plot</f>
+        <f t="shared" si="0"/>
         <v>6.4349999999999996</v>
       </c>
       <c r="H3">
-        <f>F3/Scale_plot</f>
+        <f t="shared" si="1"/>
         <v>37.089337175792508</v>
       </c>
     </row>
@@ -6335,19 +6336,19 @@
         <v>127.4</v>
       </c>
       <c r="E4">
+        <f t="shared" si="2"/>
+        <v>127.4</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="3"/>
+        <v>646.70050761421317</v>
+      </c>
+      <c r="G4">
         <f t="shared" si="0"/>
-        <v>127.4</v>
-      </c>
-      <c r="F4">
+        <v>12.74</v>
+      </c>
+      <c r="H4">
         <f t="shared" si="1"/>
-        <v>646.70050761421317</v>
-      </c>
-      <c r="G4">
-        <f>E4/Scale_plot</f>
-        <v>12.74</v>
-      </c>
-      <c r="H4">
-        <f>F4/Scale_plot</f>
         <v>64.670050761421322</v>
       </c>
     </row>
@@ -6368,19 +6369,19 @@
         <v>126.1</v>
       </c>
       <c r="E5">
+        <f t="shared" si="2"/>
+        <v>189.14999999999998</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="3"/>
+        <v>857.82312925170061</v>
+      </c>
+      <c r="G5">
         <f t="shared" si="0"/>
-        <v>189.14999999999998</v>
-      </c>
-      <c r="F5">
+        <v>18.914999999999999</v>
+      </c>
+      <c r="H5">
         <f t="shared" si="1"/>
-        <v>857.82312925170061</v>
-      </c>
-      <c r="G5">
-        <f>E5/Scale_plot</f>
-        <v>18.914999999999999</v>
-      </c>
-      <c r="H5">
-        <f>F5/Scale_plot</f>
         <v>85.782312925170061</v>
       </c>
     </row>
@@ -6401,19 +6402,19 @@
         <v>124.8</v>
       </c>
       <c r="E6">
+        <f t="shared" si="2"/>
+        <v>249.6</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="3"/>
+        <v>1022.9508196721312</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="0"/>
-        <v>249.6</v>
-      </c>
-      <c r="F6">
+        <v>24.96</v>
+      </c>
+      <c r="H6">
         <f t="shared" si="1"/>
-        <v>1022.9508196721312</v>
-      </c>
-      <c r="G6">
-        <f>E6/Scale_plot</f>
-        <v>24.96</v>
-      </c>
-      <c r="H6">
-        <f>F6/Scale_plot</f>
         <v>102.29508196721312</v>
       </c>
     </row>
@@ -6434,19 +6435,19 @@
         <v>123.5</v>
       </c>
       <c r="E7">
+        <f t="shared" si="2"/>
+        <v>308.75</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="3"/>
+        <v>1154.2056074766356</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="0"/>
-        <v>308.75</v>
-      </c>
-      <c r="F7">
+        <v>30.875</v>
+      </c>
+      <c r="H7">
         <f t="shared" si="1"/>
-        <v>1154.2056074766356</v>
-      </c>
-      <c r="G7">
-        <f>E7/Scale_plot</f>
-        <v>30.875</v>
-      </c>
-      <c r="H7">
-        <f>F7/Scale_plot</f>
         <v>115.42056074766356</v>
       </c>
     </row>
@@ -6467,19 +6468,19 @@
         <v>122.2</v>
       </c>
       <c r="E8">
+        <f t="shared" si="2"/>
+        <v>366.6</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="3"/>
+        <v>1259.7938144329896</v>
+      </c>
+      <c r="G8">
         <f t="shared" si="0"/>
-        <v>366.6</v>
-      </c>
-      <c r="F8">
+        <v>36.660000000000004</v>
+      </c>
+      <c r="H8">
         <f t="shared" si="1"/>
-        <v>1259.7938144329896</v>
-      </c>
-      <c r="G8">
-        <f>E8/Scale_plot</f>
-        <v>36.660000000000004</v>
-      </c>
-      <c r="H8">
-        <f>F8/Scale_plot</f>
         <v>125.97938144329896</v>
       </c>
     </row>
@@ -6500,19 +6501,19 @@
         <v>120.9</v>
       </c>
       <c r="E9">
+        <f t="shared" si="2"/>
+        <v>423.15000000000003</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="3"/>
+        <v>1345.4689984101749</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="0"/>
-        <v>423.15000000000003</v>
-      </c>
-      <c r="F9">
+        <v>42.315000000000005</v>
+      </c>
+      <c r="H9">
         <f t="shared" si="1"/>
-        <v>1345.4689984101749</v>
-      </c>
-      <c r="G9">
-        <f>E9/Scale_plot</f>
-        <v>42.315000000000005</v>
-      </c>
-      <c r="H9">
-        <f>F9/Scale_plot</f>
         <v>134.54689984101748</v>
       </c>
     </row>
@@ -6533,19 +6534,19 @@
         <v>119.6</v>
       </c>
       <c r="E10">
+        <f t="shared" si="2"/>
+        <v>478.4</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="3"/>
+        <v>1415.3846153846155</v>
+      </c>
+      <c r="G10">
         <f t="shared" si="0"/>
-        <v>478.4</v>
-      </c>
-      <c r="F10">
+        <v>47.839999999999996</v>
+      </c>
+      <c r="H10">
         <f t="shared" si="1"/>
-        <v>1415.3846153846155</v>
-      </c>
-      <c r="G10">
-        <f>E10/Scale_plot</f>
-        <v>47.839999999999996</v>
-      </c>
-      <c r="H10">
-        <f>F10/Scale_plot</f>
         <v>141.53846153846155</v>
       </c>
     </row>
@@ -6566,19 +6567,19 @@
         <v>118.3</v>
       </c>
       <c r="E11">
+        <f t="shared" si="2"/>
+        <v>532.35</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>1472.6141078838175</v>
+      </c>
+      <c r="G11">
         <f t="shared" si="0"/>
-        <v>532.35</v>
-      </c>
-      <c r="F11">
+        <v>53.234999999999999</v>
+      </c>
+      <c r="H11">
         <f t="shared" si="1"/>
-        <v>1472.6141078838175</v>
-      </c>
-      <c r="G11">
-        <f>E11/Scale_plot</f>
-        <v>53.234999999999999</v>
-      </c>
-      <c r="H11">
-        <f>F11/Scale_plot</f>
         <v>147.26141078838174</v>
       </c>
     </row>
@@ -6599,19 +6600,19 @@
         <v>117</v>
       </c>
       <c r="E12">
+        <f t="shared" si="2"/>
+        <v>585</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="3"/>
+        <v>1519.4805194805194</v>
+      </c>
+      <c r="G12">
         <f t="shared" si="0"/>
-        <v>585</v>
-      </c>
-      <c r="F12">
+        <v>58.5</v>
+      </c>
+      <c r="H12">
         <f t="shared" si="1"/>
-        <v>1519.4805194805194</v>
-      </c>
-      <c r="G12">
-        <f>E12/Scale_plot</f>
-        <v>58.5</v>
-      </c>
-      <c r="H12">
-        <f>F12/Scale_plot</f>
         <v>151.94805194805195</v>
       </c>
     </row>
@@ -6632,19 +6633,19 @@
         <v>115.7</v>
       </c>
       <c r="E13">
+        <f t="shared" si="2"/>
+        <v>636.35</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>1557.7723378212977</v>
+      </c>
+      <c r="G13">
         <f t="shared" si="0"/>
-        <v>636.35</v>
-      </c>
-      <c r="F13">
+        <v>63.635000000000005</v>
+      </c>
+      <c r="H13">
         <f t="shared" si="1"/>
-        <v>1557.7723378212977</v>
-      </c>
-      <c r="G13">
-        <f>E13/Scale_plot</f>
-        <v>63.635000000000005</v>
-      </c>
-      <c r="H13">
-        <f>F13/Scale_plot</f>
         <v>155.77723378212977</v>
       </c>
     </row>
@@ -6665,19 +6666,19 @@
         <v>114.4</v>
       </c>
       <c r="E14">
+        <f t="shared" si="2"/>
+        <v>686.40000000000009</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>1588.8888888888889</v>
+      </c>
+      <c r="G14">
         <f t="shared" si="0"/>
-        <v>686.40000000000009</v>
-      </c>
-      <c r="F14">
+        <v>68.640000000000015</v>
+      </c>
+      <c r="H14">
         <f t="shared" si="1"/>
-        <v>1588.8888888888889</v>
-      </c>
-      <c r="G14">
-        <f>E14/Scale_plot</f>
-        <v>68.640000000000015</v>
-      </c>
-      <c r="H14">
-        <f>F14/Scale_plot</f>
         <v>158.88888888888889</v>
       </c>
     </row>
@@ -6698,19 +6699,19 @@
         <v>113.1</v>
       </c>
       <c r="E15">
+        <f t="shared" si="2"/>
+        <v>735.15</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="3"/>
+        <v>1613.9407244785948</v>
+      </c>
+      <c r="G15">
         <f t="shared" si="0"/>
-        <v>735.15</v>
-      </c>
-      <c r="F15">
+        <v>73.515000000000001</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="1"/>
-        <v>1613.9407244785948</v>
-      </c>
-      <c r="G15">
-        <f>E15/Scale_plot</f>
-        <v>73.515000000000001</v>
-      </c>
-      <c r="H15">
-        <f>F15/Scale_plot</f>
         <v>161.39407244785949</v>
       </c>
     </row>
@@ -6731,19 +6732,19 @@
         <v>111.8</v>
       </c>
       <c r="E16">
+        <f t="shared" si="2"/>
+        <v>782.6</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>1633.820459290188</v>
+      </c>
+      <c r="G16">
         <f t="shared" si="0"/>
-        <v>782.6</v>
-      </c>
-      <c r="F16">
+        <v>78.260000000000005</v>
+      </c>
+      <c r="H16">
         <f t="shared" si="1"/>
-        <v>1633.820459290188</v>
-      </c>
-      <c r="G16">
-        <f>E16/Scale_plot</f>
-        <v>78.260000000000005</v>
-      </c>
-      <c r="H16">
-        <f>F16/Scale_plot</f>
         <v>163.3820459290188</v>
       </c>
     </row>
@@ -6764,19 +6765,19 @@
         <v>110.5</v>
       </c>
       <c r="E17">
+        <f t="shared" si="2"/>
+        <v>828.75</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>1649.2537313432838</v>
+      </c>
+      <c r="G17">
         <f t="shared" si="0"/>
-        <v>828.75</v>
-      </c>
-      <c r="F17">
+        <v>82.875</v>
+      </c>
+      <c r="H17">
         <f t="shared" si="1"/>
-        <v>1649.2537313432838</v>
-      </c>
-      <c r="G17">
-        <f>E17/Scale_plot</f>
-        <v>82.875</v>
-      </c>
-      <c r="H17">
-        <f>F17/Scale_plot</f>
         <v>164.92537313432837</v>
       </c>
     </row>
@@ -6797,19 +6798,19 @@
         <v>109.2</v>
       </c>
       <c r="E18">
+        <f t="shared" si="2"/>
+        <v>873.6</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>1660.8365019011408</v>
+      </c>
+      <c r="G18">
         <f t="shared" si="0"/>
-        <v>873.6</v>
-      </c>
-      <c r="F18">
+        <v>87.36</v>
+      </c>
+      <c r="H18">
         <f t="shared" si="1"/>
-        <v>1660.8365019011408</v>
-      </c>
-      <c r="G18">
-        <f>E18/Scale_plot</f>
-        <v>87.36</v>
-      </c>
-      <c r="H18">
-        <f>F18/Scale_plot</f>
         <v>166.08365019011407</v>
       </c>
     </row>
@@ -6830,19 +6831,19 @@
         <v>107.9</v>
       </c>
       <c r="E19">
+        <f t="shared" si="2"/>
+        <v>917.15000000000009</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>1669.0627843494087</v>
+      </c>
+      <c r="G19">
         <f t="shared" si="0"/>
-        <v>917.15000000000009</v>
-      </c>
-      <c r="F19">
+        <v>91.715000000000003</v>
+      </c>
+      <c r="H19">
         <f t="shared" si="1"/>
-        <v>1669.0627843494087</v>
-      </c>
-      <c r="G19">
-        <f>E19/Scale_plot</f>
-        <v>91.715000000000003</v>
-      </c>
-      <c r="H19">
-        <f>F19/Scale_plot</f>
         <v>166.90627843494087</v>
       </c>
     </row>
@@ -6863,19 +6864,19 @@
         <v>106.6</v>
       </c>
       <c r="E20">
+        <f t="shared" si="2"/>
+        <v>959.4</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>1674.3455497382199</v>
+      </c>
+      <c r="G20">
         <f t="shared" si="0"/>
-        <v>959.4</v>
-      </c>
-      <c r="F20">
+        <v>95.94</v>
+      </c>
+      <c r="H20">
         <f t="shared" si="1"/>
-        <v>1674.3455497382199</v>
-      </c>
-      <c r="G20">
-        <f>E20/Scale_plot</f>
-        <v>95.94</v>
-      </c>
-      <c r="H20">
-        <f>F20/Scale_plot</f>
         <v>167.434554973822</v>
       </c>
     </row>
@@ -6896,19 +6897,19 @@
         <v>105.3</v>
       </c>
       <c r="E21">
+        <f t="shared" si="2"/>
+        <v>1000.35</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="3"/>
+        <v>1677.032690695725</v>
+      </c>
+      <c r="G21">
         <f t="shared" si="0"/>
-        <v>1000.35</v>
-      </c>
-      <c r="F21">
+        <v>100.035</v>
+      </c>
+      <c r="H21">
         <f t="shared" si="1"/>
-        <v>1677.032690695725</v>
-      </c>
-      <c r="G21">
-        <f>E21/Scale_plot</f>
-        <v>100.035</v>
-      </c>
-      <c r="H21">
-        <f>F21/Scale_plot</f>
         <v>167.70326906957251</v>
       </c>
     </row>
@@ -6929,19 +6930,19 @@
         <v>104</v>
       </c>
       <c r="E22">
+        <f t="shared" si="2"/>
+        <v>1040</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="3"/>
+        <v>1677.4193548387098</v>
+      </c>
+      <c r="G22">
         <f t="shared" si="0"/>
-        <v>1040</v>
-      </c>
-      <c r="F22">
+        <v>104</v>
+      </c>
+      <c r="H22">
         <f t="shared" si="1"/>
-        <v>1677.4193548387098</v>
-      </c>
-      <c r="G22">
-        <f>E22/Scale_plot</f>
-        <v>104</v>
-      </c>
-      <c r="H22">
-        <f>F22/Scale_plot</f>
         <v>167.74193548387098</v>
       </c>
     </row>
@@ -6962,19 +6963,19 @@
         <v>102.7</v>
       </c>
       <c r="E23">
+        <f t="shared" si="2"/>
+        <v>1078.3500000000001</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="3"/>
+        <v>1675.757575757576</v>
+      </c>
+      <c r="G23">
         <f t="shared" si="0"/>
-        <v>1078.3500000000001</v>
-      </c>
-      <c r="F23">
+        <v>107.83500000000001</v>
+      </c>
+      <c r="H23">
         <f t="shared" si="1"/>
-        <v>1675.757575757576</v>
-      </c>
-      <c r="G23">
-        <f>E23/Scale_plot</f>
-        <v>107.83500000000001</v>
-      </c>
-      <c r="H23">
-        <f>F23/Scale_plot</f>
         <v>167.57575757575759</v>
       </c>
     </row>
@@ -6995,19 +6996,19 @@
         <v>101.4</v>
       </c>
       <c r="E24">
+        <f t="shared" si="2"/>
+        <v>1115.4000000000001</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="3"/>
+        <v>1672.263868065967</v>
+      </c>
+      <c r="G24">
         <f t="shared" si="0"/>
-        <v>1115.4000000000001</v>
-      </c>
-      <c r="F24">
+        <v>111.54</v>
+      </c>
+      <c r="H24">
         <f t="shared" si="1"/>
-        <v>1672.263868065967</v>
-      </c>
-      <c r="G24">
-        <f>E24/Scale_plot</f>
-        <v>111.54</v>
-      </c>
-      <c r="H24">
-        <f>F24/Scale_plot</f>
         <v>167.22638680659671</v>
       </c>
     </row>
@@ -7028,19 +7029,19 @@
         <v>100.1</v>
       </c>
       <c r="E25">
+        <f t="shared" si="2"/>
+        <v>1151.1499999999999</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="3"/>
+        <v>1667.1252715423605</v>
+      </c>
+      <c r="G25">
         <f t="shared" si="0"/>
-        <v>1151.1499999999999</v>
-      </c>
-      <c r="F25">
+        <v>115.11499999999998</v>
+      </c>
+      <c r="H25">
         <f t="shared" si="1"/>
-        <v>1667.1252715423605</v>
-      </c>
-      <c r="G25">
-        <f>E25/Scale_plot</f>
-        <v>115.11499999999998</v>
-      </c>
-      <c r="H25">
-        <f>F25/Scale_plot</f>
         <v>166.71252715423606</v>
       </c>
     </row>
@@ -7061,19 +7062,19 @@
         <v>98.8</v>
       </c>
       <c r="E26">
+        <f t="shared" si="2"/>
+        <v>1185.5999999999999</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="3"/>
+        <v>1660.5042016806719</v>
+      </c>
+      <c r="G26">
         <f t="shared" si="0"/>
-        <v>1185.5999999999999</v>
-      </c>
-      <c r="F26">
+        <v>118.55999999999999</v>
+      </c>
+      <c r="H26">
         <f t="shared" si="1"/>
-        <v>1660.5042016806719</v>
-      </c>
-      <c r="G26">
-        <f>E26/Scale_plot</f>
-        <v>118.55999999999999</v>
-      </c>
-      <c r="H26">
-        <f>F26/Scale_plot</f>
         <v>166.05042016806721</v>
       </c>
     </row>
@@ -7094,19 +7095,19 @@
         <v>97.5</v>
       </c>
       <c r="E27">
+        <f t="shared" si="2"/>
+        <v>1218.75</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="3"/>
+        <v>1652.5423728813557</v>
+      </c>
+      <c r="G27">
         <f t="shared" si="0"/>
-        <v>1218.75</v>
-      </c>
-      <c r="F27">
+        <v>121.875</v>
+      </c>
+      <c r="H27">
         <f t="shared" si="1"/>
-        <v>1652.5423728813557</v>
-      </c>
-      <c r="G27">
-        <f>E27/Scale_plot</f>
-        <v>121.875</v>
-      </c>
-      <c r="H27">
-        <f>F27/Scale_plot</f>
         <v>165.25423728813558</v>
       </c>
     </row>
@@ -7127,19 +7128,19 @@
         <v>96.199999999999989</v>
       </c>
       <c r="E28">
+        <f t="shared" si="2"/>
+        <v>1250.5999999999999</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="3"/>
+        <v>1643.363994743758</v>
+      </c>
+      <c r="G28">
         <f t="shared" si="0"/>
-        <v>1250.5999999999999</v>
-      </c>
-      <c r="F28">
+        <v>125.05999999999999</v>
+      </c>
+      <c r="H28">
         <f t="shared" si="1"/>
-        <v>1643.363994743758</v>
-      </c>
-      <c r="G28">
-        <f>E28/Scale_plot</f>
-        <v>125.05999999999999</v>
-      </c>
-      <c r="H28">
-        <f>F28/Scale_plot</f>
         <v>164.33639947437581</v>
       </c>
     </row>
@@ -7160,19 +7161,19 @@
         <v>94.9</v>
       </c>
       <c r="E29">
+        <f t="shared" si="2"/>
+        <v>1281.1500000000001</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="3"/>
+        <v>1633.0783938814534</v>
+      </c>
+      <c r="G29">
         <f t="shared" si="0"/>
-        <v>1281.1500000000001</v>
-      </c>
-      <c r="F29">
+        <v>128.11500000000001</v>
+      </c>
+      <c r="H29">
         <f t="shared" si="1"/>
-        <v>1633.0783938814534</v>
-      </c>
-      <c r="G29">
-        <f>E29/Scale_plot</f>
-        <v>128.11500000000001</v>
-      </c>
-      <c r="H29">
-        <f>F29/Scale_plot</f>
         <v>163.30783938814534</v>
       </c>
     </row>
@@ -7193,19 +7194,19 @@
         <v>93.6</v>
       </c>
       <c r="E30">
+        <f t="shared" si="2"/>
+        <v>1310.3999999999999</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="3"/>
+        <v>1621.7821782178214</v>
+      </c>
+      <c r="G30">
         <f t="shared" si="0"/>
-        <v>1310.3999999999999</v>
-      </c>
-      <c r="F30">
+        <v>131.04</v>
+      </c>
+      <c r="H30">
         <f t="shared" si="1"/>
-        <v>1621.7821782178214</v>
-      </c>
-      <c r="G30">
-        <f>E30/Scale_plot</f>
-        <v>131.04</v>
-      </c>
-      <c r="H30">
-        <f>F30/Scale_plot</f>
         <v>162.17821782178214</v>
       </c>
     </row>
@@ -7226,19 +7227,19 @@
         <v>92.3</v>
       </c>
       <c r="E31">
+        <f t="shared" si="2"/>
+        <v>1338.35</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="3"/>
+        <v>1609.5610342754057</v>
+      </c>
+      <c r="G31">
         <f t="shared" si="0"/>
-        <v>1338.35</v>
-      </c>
-      <c r="F31">
+        <v>133.83499999999998</v>
+      </c>
+      <c r="H31">
         <f t="shared" si="1"/>
-        <v>1609.5610342754057</v>
-      </c>
-      <c r="G31">
-        <f>E31/Scale_plot</f>
-        <v>133.83499999999998</v>
-      </c>
-      <c r="H31">
-        <f>F31/Scale_plot</f>
         <v>160.95610342754057</v>
       </c>
     </row>
@@ -7259,19 +7260,19 @@
         <v>91</v>
       </c>
       <c r="E32">
+        <f t="shared" si="2"/>
+        <v>1365</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="3"/>
+        <v>1596.4912280701756</v>
+      </c>
+      <c r="G32">
         <f t="shared" si="0"/>
-        <v>1365</v>
-      </c>
-      <c r="F32">
+        <v>136.5</v>
+      </c>
+      <c r="H32">
         <f t="shared" si="1"/>
-        <v>1596.4912280701756</v>
-      </c>
-      <c r="G32">
-        <f>E32/Scale_plot</f>
-        <v>136.5</v>
-      </c>
-      <c r="H32">
-        <f>F32/Scale_plot</f>
         <v>159.64912280701756</v>
       </c>
     </row>
@@ -7292,19 +7293,19 @@
         <v>89.699999999999989</v>
       </c>
       <c r="E33">
+        <f t="shared" si="2"/>
+        <v>1390.35</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="3"/>
+        <v>1582.6408651109844</v>
+      </c>
+      <c r="G33">
         <f t="shared" si="0"/>
-        <v>1390.35</v>
-      </c>
-      <c r="F33">
+        <v>139.035</v>
+      </c>
+      <c r="H33">
         <f t="shared" si="1"/>
-        <v>1582.6408651109844</v>
-      </c>
-      <c r="G33">
-        <f>E33/Scale_plot</f>
-        <v>139.035</v>
-      </c>
-      <c r="H33">
-        <f>F33/Scale_plot</f>
         <v>158.26408651109844</v>
       </c>
     </row>
@@ -7325,19 +7326,19 @@
         <v>88.4</v>
       </c>
       <c r="E34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1414.4</v>
       </c>
       <c r="F34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1568.0709534368073</v>
       </c>
       <c r="G34">
-        <f>E34/Scale_plot</f>
+        <f t="shared" ref="G34:G65" si="4">E34/Scale_plot</f>
         <v>141.44</v>
       </c>
       <c r="H34">
-        <f>F34/Scale_plot</f>
+        <f t="shared" ref="H34:H65" si="5">F34/Scale_plot</f>
         <v>156.80709534368071</v>
       </c>
     </row>
@@ -7358,19 +7359,19 @@
         <v>87.1</v>
       </c>
       <c r="E35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1437.1499999999999</v>
       </c>
       <c r="F35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1552.8363047001619</v>
       </c>
       <c r="G35">
-        <f>E35/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>143.71499999999997</v>
       </c>
       <c r="H35">
-        <f>F35/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>155.28363047001619</v>
       </c>
     </row>
@@ -7391,19 +7392,19 @@
         <v>85.8</v>
       </c>
       <c r="E36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1458.6</v>
       </c>
       <c r="F36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1536.9863013698628</v>
       </c>
       <c r="G36">
-        <f>E36/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>145.85999999999999</v>
       </c>
       <c r="H36">
-        <f>F36/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>153.69863013698628</v>
       </c>
     </row>
@@ -7424,19 +7425,19 @@
         <v>84.5</v>
       </c>
       <c r="E37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1478.75</v>
       </c>
       <c r="F37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1520.5655526992286</v>
       </c>
       <c r="G37">
-        <f>E37/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>147.875</v>
       </c>
       <c r="H37">
-        <f>F37/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>152.05655526992285</v>
       </c>
     </row>
@@ -7457,19 +7458,19 @@
         <v>83.199999999999989</v>
       </c>
       <c r="E38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1497.6</v>
       </c>
       <c r="F38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1503.6144578313251</v>
       </c>
       <c r="G38">
-        <f>E38/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>149.76</v>
       </c>
       <c r="H38">
-        <f>F38/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>150.36144578313252</v>
       </c>
     </row>
@@ -7490,19 +7491,19 @@
         <v>81.900000000000006</v>
       </c>
       <c r="E39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1515.15</v>
       </c>
       <c r="F39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1486.1696910250123</v>
       </c>
       <c r="G39">
-        <f>E39/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>151.51500000000001</v>
       </c>
       <c r="H39">
-        <f>F39/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>148.61696910250123</v>
       </c>
     </row>
@@ -7523,19 +7524,19 @@
         <v>80.599999999999994</v>
       </c>
       <c r="E40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1531.3999999999999</v>
       </c>
       <c r="F40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1468.2646212847555</v>
       </c>
       <c r="G40">
-        <f>E40/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>153.13999999999999</v>
       </c>
       <c r="H40">
-        <f>F40/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>146.82646212847555</v>
       </c>
     </row>
@@ -7556,19 +7557,19 @@
         <v>79.3</v>
       </c>
       <c r="E41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1546.35</v>
       </c>
       <c r="F41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1449.929676511955</v>
       </c>
       <c r="G41">
-        <f>E41/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>154.63499999999999</v>
       </c>
       <c r="H41">
-        <f>F41/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>144.9929676511955</v>
       </c>
     </row>
@@ -7589,19 +7590,19 @@
         <v>78</v>
       </c>
       <c r="E42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1560</v>
       </c>
       <c r="F42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1431.1926605504589</v>
       </c>
       <c r="G42">
-        <f>E42/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>156</v>
       </c>
       <c r="H42">
-        <f>F42/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>143.1192660550459</v>
       </c>
     </row>
@@ -7622,19 +7623,19 @@
         <v>76.699999999999989</v>
       </c>
       <c r="E43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1572.3499999999997</v>
       </c>
       <c r="F43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1412.0790300853164</v>
       </c>
       <c r="G43">
-        <f>E43/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>157.23499999999996</v>
       </c>
       <c r="H43">
-        <f>F43/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>141.20790300853164</v>
       </c>
     </row>
@@ -7655,19 +7656,19 @@
         <v>75.400000000000006</v>
       </c>
       <c r="E44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1583.4</v>
       </c>
       <c r="F44">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1392.6121372031662</v>
       </c>
       <c r="G44">
-        <f>E44/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>158.34</v>
       </c>
       <c r="H44">
-        <f>F44/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>139.26121372031662</v>
       </c>
     </row>
@@ -7688,19 +7689,19 @@
         <v>74.099999999999994</v>
       </c>
       <c r="E45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1593.1499999999999</v>
       </c>
       <c r="F45">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1372.813442481689</v>
       </c>
       <c r="G45">
-        <f>E45/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>159.315</v>
       </c>
       <c r="H45">
-        <f>F45/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>137.28134424816889</v>
       </c>
     </row>
@@ -7721,19 +7722,19 @@
         <v>72.8</v>
       </c>
       <c r="E46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1601.6</v>
       </c>
       <c r="F46">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1352.7027027027027</v>
       </c>
       <c r="G46">
-        <f>E46/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>160.16</v>
       </c>
       <c r="H46">
-        <f>F46/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>135.27027027027026</v>
       </c>
     </row>
@@ -7754,19 +7755,19 @@
         <v>71.5</v>
       </c>
       <c r="E47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1608.75</v>
       </c>
       <c r="F47">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1332.2981366459628</v>
       </c>
       <c r="G47">
-        <f>E47/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>160.875</v>
       </c>
       <c r="H47">
-        <f>F47/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>133.22981366459629</v>
       </c>
     </row>
@@ -7787,19 +7788,19 @@
         <v>70.199999999999989</v>
       </c>
       <c r="E48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1614.5999999999997</v>
       </c>
       <c r="F48">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1311.61657189277</v>
       </c>
       <c r="G48">
-        <f>E48/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>161.45999999999998</v>
       </c>
       <c r="H48">
-        <f>F48/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>131.16165718927701</v>
       </c>
     </row>
@@ -7820,19 +7821,19 @@
         <v>68.900000000000006</v>
       </c>
       <c r="E49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1619.15</v>
       </c>
       <c r="F49">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1290.6735751295339</v>
       </c>
       <c r="G49">
-        <f>E49/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>161.91500000000002</v>
       </c>
       <c r="H49">
-        <f>F49/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>129.06735751295338</v>
       </c>
     </row>
@@ -7853,19 +7854,19 @@
         <v>67.599999999999994</v>
       </c>
       <c r="E50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1622.3999999999999</v>
       </c>
       <c r="F50">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1269.4835680751173</v>
       </c>
       <c r="G50">
-        <f>E50/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>162.23999999999998</v>
       </c>
       <c r="H50">
-        <f>F50/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>126.94835680751173</v>
       </c>
     </row>
@@ -7886,19 +7887,19 @@
         <v>66.3</v>
       </c>
       <c r="E51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1624.35</v>
       </c>
       <c r="F51">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1248.0599308490205</v>
       </c>
       <c r="G51">
-        <f>E51/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>162.435</v>
       </c>
       <c r="H51">
-        <f>F51/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>124.80599308490204</v>
       </c>
     </row>
@@ -7919,19 +7920,19 @@
         <v>65</v>
       </c>
       <c r="E52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1625</v>
       </c>
       <c r="F52">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1226.4150943396228</v>
       </c>
       <c r="G52">
-        <f>E52/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>162.5</v>
       </c>
       <c r="H52">
-        <f>F52/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>122.64150943396228</v>
       </c>
     </row>
@@ -7952,19 +7953,19 @@
         <v>63.7</v>
       </c>
       <c r="E53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1624.3500000000001</v>
       </c>
       <c r="F53">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1204.5606229143496</v>
       </c>
       <c r="G53">
-        <f>E53/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>162.435</v>
       </c>
       <c r="H53">
-        <f>F53/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>120.45606229143496</v>
       </c>
     </row>
@@ -7985,19 +7986,19 @@
         <v>62.399999999999991</v>
       </c>
       <c r="E54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1622.3999999999999</v>
       </c>
       <c r="F54">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1182.5072886297376</v>
       </c>
       <c r="G54">
-        <f>E54/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>162.23999999999998</v>
       </c>
       <c r="H54">
-        <f>F54/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>118.25072886297376</v>
       </c>
     </row>
@@ -8018,19 +8019,19 @@
         <v>61.099999999999994</v>
       </c>
       <c r="E55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1619.1499999999999</v>
       </c>
       <c r="F55">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1160.2651379433894</v>
       </c>
       <c r="G55">
-        <f>E55/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>161.91499999999999</v>
       </c>
       <c r="H55">
-        <f>F55/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>116.02651379433894</v>
       </c>
     </row>
@@ -8051,19 +8052,19 @@
         <v>59.8</v>
       </c>
       <c r="E56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1614.6</v>
       </c>
       <c r="F56">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1137.8435517970402</v>
       </c>
       <c r="G56">
-        <f>E56/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>161.45999999999998</v>
       </c>
       <c r="H56">
-        <f>F56/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>113.78435517970402</v>
       </c>
     </row>
@@ -8084,19 +8085,19 @@
         <v>58.5</v>
       </c>
       <c r="E57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1608.75</v>
       </c>
       <c r="F57">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1115.2512998266898</v>
       </c>
       <c r="G57">
-        <f>E57/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>160.875</v>
       </c>
       <c r="H57">
-        <f>F57/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>111.52512998266897</v>
       </c>
     </row>
@@ -8117,19 +8118,19 @@
         <v>57.2</v>
       </c>
       <c r="E58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1601.6000000000001</v>
       </c>
       <c r="F58">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1092.4965893587996</v>
       </c>
       <c r="G58">
-        <f>E58/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>160.16000000000003</v>
       </c>
       <c r="H58">
-        <f>F58/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>109.24965893587996</v>
       </c>
     </row>
@@ -8150,19 +8151,19 @@
         <v>55.899999999999991</v>
       </c>
       <c r="E59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1593.1499999999999</v>
       </c>
       <c r="F59">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1069.5871097683787</v>
       </c>
       <c r="G59">
-        <f>E59/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>159.315</v>
       </c>
       <c r="H59">
-        <f>F59/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>106.95871097683786</v>
       </c>
     </row>
@@ -8183,19 +8184,19 @@
         <v>54.599999999999994</v>
       </c>
       <c r="E60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1583.3999999999999</v>
       </c>
       <c r="F60">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1046.5300727032386</v>
       </c>
       <c r="G60">
-        <f>E60/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>158.33999999999997</v>
       </c>
       <c r="H60">
-        <f>F60/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>104.65300727032385</v>
       </c>
     </row>
@@ -8216,19 +8217,19 @@
         <v>53.3</v>
       </c>
       <c r="E61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1572.35</v>
       </c>
       <c r="F61">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1023.3322486169866</v>
       </c>
       <c r="G61">
-        <f>E61/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>157.23499999999999</v>
       </c>
       <c r="H61">
-        <f>F61/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>102.33322486169865</v>
       </c>
     </row>
@@ -8249,19 +8250,19 @@
         <v>52</v>
       </c>
       <c r="E62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1560</v>
       </c>
       <c r="F62">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1000.0000000000001</v>
       </c>
       <c r="G62">
-        <f>E62/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>156</v>
       </c>
       <c r="H62">
-        <f>F62/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>100.00000000000001</v>
       </c>
     </row>
@@ -8282,19 +8283,19 @@
         <v>50.7</v>
       </c>
       <c r="E63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1546.3500000000001</v>
       </c>
       <c r="F63">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>976.53931165140523</v>
       </c>
       <c r="G63">
-        <f>E63/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>154.63500000000002</v>
       </c>
       <c r="H63">
-        <f>F63/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>97.65393116514052</v>
       </c>
     </row>
@@ -8315,19 +8316,19 @@
         <v>49.399999999999991</v>
       </c>
       <c r="E64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1531.3999999999996</v>
       </c>
       <c r="F64">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>952.95581829495939</v>
       </c>
       <c r="G64">
-        <f>E64/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>153.13999999999996</v>
       </c>
       <c r="H64">
-        <f>F64/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>95.295581829495944</v>
       </c>
     </row>
@@ -8348,19 +8349,19 @@
         <v>48.099999999999994</v>
       </c>
       <c r="E65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1515.1499999999999</v>
       </c>
       <c r="F65">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>929.25482980680772</v>
       </c>
       <c r="G65">
-        <f>E65/Scale_plot</f>
+        <f t="shared" si="4"/>
         <v>151.51499999999999</v>
       </c>
       <c r="H65">
-        <f>F65/Scale_plot</f>
+        <f t="shared" si="5"/>
         <v>92.925482980680769</v>
       </c>
     </row>
@@ -8381,19 +8382,19 @@
         <v>46.8</v>
       </c>
       <c r="E66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1497.6</v>
       </c>
       <c r="F66">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>905.44135429262394</v>
       </c>
       <c r="G66">
-        <f>E66/Scale_plot</f>
+        <f t="shared" ref="G66:G102" si="6">E66/Scale_plot</f>
         <v>149.76</v>
       </c>
       <c r="H66">
-        <f>F66/Scale_plot</f>
+        <f t="shared" ref="H66:H102" si="7">F66/Scale_plot</f>
         <v>90.544135429262397</v>
       </c>
     </row>
@@ -8414,19 +8415,19 @@
         <v>45.5</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E102" si="2">B67*D67</f>
+        <f t="shared" ref="E67:E102" si="8">B67*D67</f>
         <v>1478.75</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67:F102" si="3">E67/C67</f>
+        <f t="shared" ref="F67:F102" si="9">E67/C67</f>
         <v>881.52011922503721</v>
       </c>
       <c r="G67">
-        <f>E67/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>147.875</v>
       </c>
       <c r="H67">
-        <f>F67/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>88.152011922503718</v>
       </c>
     </row>
@@ -8447,19 +8448,19 @@
         <v>44.2</v>
       </c>
       <c r="E68">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1458.6000000000001</v>
       </c>
       <c r="F68">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>857.49559082892426</v>
       </c>
       <c r="G68">
-        <f>E68/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>145.86000000000001</v>
       </c>
       <c r="H68">
-        <f>F68/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>85.749559082892432</v>
       </c>
     </row>
@@ -8480,19 +8481,19 @@
         <v>42.899999999999991</v>
       </c>
       <c r="E69">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1437.1499999999996</v>
       </c>
       <c r="F69">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>833.37199188170462</v>
       </c>
       <c r="G69">
-        <f>E69/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>143.71499999999997</v>
       </c>
       <c r="H69">
-        <f>F69/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>83.337199188170459</v>
       </c>
     </row>
@@ -8513,19 +8514,19 @@
         <v>41.599999999999994</v>
       </c>
       <c r="E70">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1414.3999999999999</v>
       </c>
       <c r="F70">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>809.15331807780308</v>
       </c>
       <c r="G70">
-        <f>E70/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>141.44</v>
       </c>
       <c r="H70">
-        <f>F70/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>80.915331807780305</v>
       </c>
     </row>
@@ -8546,19 +8547,19 @@
         <v>40.299999999999997</v>
       </c>
       <c r="E71">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1390.35</v>
       </c>
       <c r="F71">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>784.84335309060123</v>
       </c>
       <c r="G71">
-        <f>E71/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>139.035</v>
       </c>
       <c r="H71">
-        <f>F71/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>78.484335309060128</v>
       </c>
     </row>
@@ -8579,19 +8580,19 @@
         <v>39</v>
       </c>
       <c r="E72">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1365</v>
       </c>
       <c r="F72">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>760.44568245125356</v>
       </c>
       <c r="G72">
-        <f>E72/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>136.5</v>
       </c>
       <c r="H72">
-        <f>F72/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>76.044568245125362</v>
       </c>
     </row>
@@ -8612,19 +8613,19 @@
         <v>37.700000000000003</v>
       </c>
       <c r="E73">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1338.3500000000001</v>
       </c>
       <c r="F73">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>735.96370635138862</v>
       </c>
       <c r="G73">
-        <f>E73/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>133.83500000000001</v>
       </c>
       <c r="H73">
-        <f>F73/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>73.596370635138868</v>
       </c>
     </row>
@@ -8645,19 +8646,19 @@
         <v>36.399999999999991</v>
       </c>
       <c r="E74">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1310.3999999999996</v>
       </c>
       <c r="F74">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>711.40065146579786</v>
       </c>
       <c r="G74">
-        <f>E74/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>131.03999999999996</v>
       </c>
       <c r="H74">
-        <f>F74/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>71.140065146579786</v>
       </c>
     </row>
@@ -8678,19 +8679,19 @@
         <v>35.099999999999994</v>
       </c>
       <c r="E75">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1281.1499999999999</v>
       </c>
       <c r="F75">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>686.75958188153299</v>
       </c>
       <c r="G75">
-        <f>E75/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>128.11499999999998</v>
       </c>
       <c r="H75">
-        <f>F75/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>68.675958188153302</v>
       </c>
     </row>
@@ -8711,19 +8712,19 @@
         <v>33.799999999999997</v>
       </c>
       <c r="E76">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1250.5999999999999</v>
       </c>
       <c r="F76">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>662.04340921122287</v>
       </c>
       <c r="G76">
-        <f>E76/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>125.05999999999999</v>
       </c>
       <c r="H76">
-        <f>F76/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>66.204340921122281</v>
       </c>
     </row>
@@ -8744,19 +8745,19 @@
         <v>32.5</v>
       </c>
       <c r="E77">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1218.75</v>
       </c>
       <c r="F77">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>637.25490196078431</v>
       </c>
       <c r="G77">
-        <f>E77/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>121.875</v>
       </c>
       <c r="H77">
-        <f>F77/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>63.725490196078432</v>
       </c>
     </row>
@@ -8777,19 +8778,19 @@
         <v>31.200000000000003</v>
       </c>
       <c r="E78">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1185.6000000000001</v>
       </c>
       <c r="F78">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>612.39669421487611</v>
       </c>
       <c r="G78">
-        <f>E78/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>118.56000000000002</v>
       </c>
       <c r="H78">
-        <f>F78/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>61.239669421487612</v>
       </c>
     </row>
@@ -8810,19 +8811,19 @@
         <v>29.899999999999991</v>
       </c>
       <c r="E79">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1151.1499999999996</v>
       </c>
       <c r="F79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>587.47129369737161</v>
       </c>
       <c r="G79">
-        <f>E79/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>115.11499999999997</v>
       </c>
       <c r="H79">
-        <f>F79/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>58.747129369737159</v>
       </c>
     </row>
@@ -8843,19 +8844,19 @@
         <v>28.599999999999994</v>
       </c>
       <c r="E80">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1115.3999999999999</v>
       </c>
       <c r="F80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>562.48108925869894</v>
       </c>
       <c r="G80">
-        <f>E80/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>111.53999999999999</v>
       </c>
       <c r="H80">
-        <f>F80/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>56.248108925869893</v>
       </c>
     </row>
@@ -8876,19 +8877,19 @@
         <v>27.299999999999997</v>
       </c>
       <c r="E81">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1078.3499999999999</v>
       </c>
       <c r="F81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>537.42835783702958</v>
       </c>
       <c r="G81">
-        <f>E81/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>107.83499999999999</v>
       </c>
       <c r="H81">
-        <f>F81/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>53.742835783702958</v>
       </c>
     </row>
@@ -8909,19 +8910,19 @@
         <v>26</v>
       </c>
       <c r="E82">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1040</v>
       </c>
       <c r="F82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>512.3152709359606</v>
       </c>
       <c r="G82">
-        <f>E82/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>104</v>
       </c>
       <c r="H82">
-        <f>F82/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>51.231527093596057</v>
       </c>
     </row>
@@ -8942,19 +8943,19 @@
         <v>24.700000000000003</v>
       </c>
       <c r="E83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>1000.3500000000001</v>
       </c>
       <c r="F83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>487.14390065741424</v>
       </c>
       <c r="G83">
-        <f>E83/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>100.03500000000001</v>
       </c>
       <c r="H83">
-        <f>F83/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>48.714390065741426</v>
       </c>
     </row>
@@ -8975,19 +8976,19 @@
         <v>23.399999999999991</v>
       </c>
       <c r="E84">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>959.39999999999964</v>
       </c>
       <c r="F84">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>461.91622532498781</v>
       </c>
       <c r="G84">
-        <f>E84/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>95.939999999999969</v>
       </c>
       <c r="H84">
-        <f>F84/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>46.191622532498783</v>
       </c>
     </row>
@@ -9008,19 +9009,19 @@
         <v>22.099999999999994</v>
       </c>
       <c r="E85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>917.14999999999975</v>
       </c>
       <c r="F85">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>436.63413472982614</v>
       </c>
       <c r="G85">
-        <f>E85/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>91.714999999999975</v>
       </c>
       <c r="H85">
-        <f>F85/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>43.663413472982612</v>
       </c>
     </row>
@@ -9041,19 +9042,19 @@
         <v>20.799999999999997</v>
       </c>
       <c r="E86">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>873.59999999999991</v>
       </c>
       <c r="F86">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>411.29943502824852</v>
       </c>
       <c r="G86">
-        <f>E86/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>87.359999999999985</v>
       </c>
       <c r="H86">
-        <f>F86/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>41.129943502824851</v>
       </c>
     </row>
@@ -9074,19 +9075,19 @@
         <v>19.5</v>
       </c>
       <c r="E87">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>828.75</v>
       </c>
       <c r="F87">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>385.9138533178114</v>
       </c>
       <c r="G87">
-        <f>E87/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>82.875</v>
       </c>
       <c r="H87">
-        <f>F87/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>38.59138533178114</v>
       </c>
     </row>
@@ -9107,19 +9108,19 @@
         <v>18.200000000000003</v>
       </c>
       <c r="E88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>782.60000000000014</v>
       </c>
       <c r="F88">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>360.47904191616777</v>
       </c>
       <c r="G88">
-        <f>E88/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>78.260000000000019</v>
       </c>
       <c r="H88">
-        <f>F88/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>36.04790419161678</v>
       </c>
     </row>
@@ -9140,19 +9141,19 @@
         <v>16.899999999999991</v>
       </c>
       <c r="E89">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>735.14999999999964</v>
       </c>
       <c r="F89">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>334.99658236500323</v>
       </c>
       <c r="G89">
-        <f>E89/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>73.514999999999958</v>
       </c>
       <c r="H89">
-        <f>F89/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>33.499658236500323</v>
       </c>
     </row>
@@ -9173,19 +9174,19 @@
         <v>15.599999999999994</v>
       </c>
       <c r="E90">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>686.39999999999975</v>
       </c>
       <c r="F90">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>309.46798917944085</v>
       </c>
       <c r="G90">
-        <f>E90/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>68.639999999999972</v>
       </c>
       <c r="H90">
-        <f>F90/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>30.946798917944086</v>
       </c>
     </row>
@@ -9206,19 +9207,19 @@
         <v>14.299999999999997</v>
       </c>
       <c r="E91">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>636.34999999999991</v>
       </c>
       <c r="F91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>283.89471336158823</v>
       </c>
       <c r="G91">
-        <f>E91/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>63.634999999999991</v>
       </c>
       <c r="H91">
-        <f>F91/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>28.389471336158824</v>
       </c>
     </row>
@@ -9239,19 +9240,19 @@
         <v>13</v>
       </c>
       <c r="E92">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>585</v>
       </c>
       <c r="F92">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>258.27814569536423</v>
       </c>
       <c r="G92">
-        <f>E92/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>58.5</v>
       </c>
       <c r="H92">
-        <f>F92/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>25.827814569536422</v>
       </c>
     </row>
@@ -9272,19 +9273,19 @@
         <v>11.700000000000003</v>
       </c>
       <c r="E93">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>532.35000000000014</v>
       </c>
       <c r="F93">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>232.61961983832211</v>
       </c>
       <c r="G93">
-        <f>E93/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>53.235000000000014</v>
       </c>
       <c r="H93">
-        <f>F93/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>23.261961983832212</v>
       </c>
     </row>
@@ -9305,19 +9306,19 @@
         <v>10.399999999999991</v>
       </c>
       <c r="E94">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>478.39999999999964</v>
       </c>
       <c r="F94">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>206.92041522491334</v>
       </c>
       <c r="G94">
-        <f>E94/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>47.839999999999961</v>
       </c>
       <c r="H94">
-        <f>F94/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>20.692041522491333</v>
       </c>
     </row>
@@ -9338,19 +9339,19 @@
         <v>9.0999999999999943</v>
       </c>
       <c r="E95">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>423.14999999999975</v>
       </c>
       <c r="F95">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>181.18175979447645</v>
       </c>
       <c r="G95">
-        <f>E95/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>42.314999999999976</v>
       </c>
       <c r="H95">
-        <f>F95/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>18.118175979447646</v>
       </c>
     </row>
@@ -9371,19 +9372,19 @@
         <v>7.7999999999999972</v>
       </c>
       <c r="E96">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>366.59999999999985</v>
       </c>
       <c r="F96">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>155.4048325561678</v>
       </c>
       <c r="G96">
-        <f>E96/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>36.659999999999982</v>
       </c>
       <c r="H96">
-        <f>F96/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>15.540483255616781</v>
       </c>
     </row>
@@ -9404,19 +9405,19 @@
         <v>6.5</v>
       </c>
       <c r="E97">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>308.75</v>
       </c>
       <c r="F97">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>129.59076600209863</v>
       </c>
       <c r="G97">
-        <f>E97/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>30.875</v>
       </c>
       <c r="H97">
-        <f>F97/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>12.959076600209864</v>
       </c>
     </row>
@@ -9437,19 +9438,19 @@
         <v>5.1999999999999886</v>
       </c>
       <c r="E98">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>249.59999999999945</v>
       </c>
       <c r="F98">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>103.74064837905213</v>
       </c>
       <c r="G98">
-        <f>E98/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>24.959999999999944</v>
       </c>
       <c r="H98">
-        <f>F98/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>10.374064837905212</v>
       </c>
     </row>
@@ -9470,19 +9471,19 @@
         <v>3.8999999999999915</v>
       </c>
       <c r="E99">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>189.14999999999958</v>
       </c>
       <c r="F99">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>77.855525828359575</v>
       </c>
       <c r="G99">
-        <f>E99/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>18.914999999999957</v>
       </c>
       <c r="H99">
-        <f>F99/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>7.7855525828359573</v>
       </c>
     </row>
@@ -9503,19 +9504,19 @@
         <v>2.5999999999999943</v>
       </c>
       <c r="E100">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>127.39999999999972</v>
       </c>
       <c r="F100">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>51.936404402772006</v>
       </c>
       <c r="G100">
-        <f>E100/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>12.739999999999972</v>
       </c>
       <c r="H100">
-        <f>F100/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>5.1936404402772007</v>
       </c>
     </row>
@@ -9536,19 +9537,19 @@
         <v>1.2999999999999829</v>
       </c>
       <c r="E101">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>64.349999999999156</v>
       </c>
       <c r="F101">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>25.9842519685036</v>
       </c>
       <c r="G101">
-        <f>E101/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>6.4349999999999152</v>
       </c>
       <c r="H101">
-        <f>F101/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>2.5984251968503598</v>
       </c>
     </row>
@@ -9569,19 +9570,19 @@
         <v>0</v>
       </c>
       <c r="E102">
-        <f t="shared" si="2"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="F102">
-        <f t="shared" si="3"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="G102">
-        <f>E102/Scale_plot</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="H102">
-        <f>F102/Scale_plot</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>